<commit_message>
ui updates and fixed 24 season bug
</commit_message>
<xml_diff>
--- a/PlayerToPro/data/usports_players_to_pro_summary.xlsx
+++ b/PlayerToPro/data/usports_players_to_pro_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/Desktop/Waterloo/IST/PlayerToPro/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCE44F1-C10A-BE44-9A8F-8FED3188156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE546CC-8D56-0440-81A6-486F80883B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6672" uniqueCount="2272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6672" uniqueCount="2273">
   <si>
     <t>Player</t>
   </si>
@@ -6836,6 +6836,9 @@
   </si>
   <si>
     <t>USA, Philippines, Mexico, UK, Netherlands</t>
+  </si>
+  <si>
+    <t>Achuil Lual (1)</t>
   </si>
 </sst>
 </file>
@@ -7201,8 +7204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G955"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
+      <selection activeCell="C501" sqref="C501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18806,7 +18809,7 @@
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
-        <v>1350</v>
+        <v>2272</v>
       </c>
       <c r="B506" t="s">
         <v>308</v>

</xml_diff>